<commit_message>
feat: Enhance bulk registration functionality with event filtering and status handling
</commit_message>
<xml_diff>
--- a/media/bulk_event/testing_bulk.xlsx
+++ b/media/bulk_event/testing_bulk.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cocdr\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85143AF0-1D1F-483B-AB9C-B7ACB6CB39E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CA6237A-E9AE-4EF4-BC62-F679DD9FCE08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -201,9 +201,6 @@
     <t>R</t>
   </si>
   <si>
-    <t>jtiongod@gmail.com</t>
-  </si>
-  <si>
     <t>Zapanta</t>
   </si>
   <si>
@@ -211,9 +208,6 @@
   </si>
   <si>
     <t>E</t>
-  </si>
-  <si>
-    <t>jfkdsjkfj@gmail.com</t>
   </si>
   <si>
     <t>Panoy</t>
@@ -238,6 +232,12 @@
   </si>
   <si>
     <t>if_coach</t>
+  </si>
+  <si>
+    <t>jtiongco.work@gmail.com</t>
+  </si>
+  <si>
+    <t>jordanzapanta61@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -794,8 +794,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1209"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1317,13 +1317,13 @@
         <v>46</v>
       </c>
       <c r="I15" s="12" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J15" s="11" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="K15" s="12" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="L15" s="11" t="s">
         <v>47</v>
@@ -1357,7 +1357,7 @@
         <v>50</v>
       </c>
       <c r="E16" s="19" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="F16" s="13">
         <v>99898989</v>
@@ -1400,16 +1400,16 @@
         <v>2</v>
       </c>
       <c r="B17" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="C17" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="C17" s="14" t="s">
+      <c r="D17" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="D17" s="14" t="s">
-        <v>54</v>
-      </c>
       <c r="E17" s="20" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="F17" s="14">
         <v>9989898</v>
@@ -1452,16 +1452,16 @@
         <v>3</v>
       </c>
       <c r="B18" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="D18" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="C18" s="14" t="s">
+      <c r="E18" s="20" t="s">
         <v>57</v>
-      </c>
-      <c r="D18" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="E18" s="20" t="s">
-        <v>59</v>
       </c>
       <c r="F18" s="14">
         <v>9989899</v>
@@ -36230,7 +36230,7 @@
       </c>
       <c r="C1" s="17">
         <f ca="1">NOW()</f>
-        <v>46024.892124999998</v>
+        <v>46029.961535879629</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -36290,7 +36290,7 @@
         <v>32</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1">

</xml_diff>